<commit_message>
add user story 2
</commit_message>
<xml_diff>
--- a/docs/OnMeal-Scrum.xlsx
+++ b/docs/OnMeal-Scrum.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chenc\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\OnMeal\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BC2EC5E-7CFC-460E-A429-A931AD11A4A5}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D03F6BA-CAFE-4E47-8018-902214637913}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4860" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <sheet name="Archives" sheetId="4" r:id="rId4"/>
     <sheet name="Burndown Chart" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -258,7 +258,7 @@
     <author>陈程</author>
   </authors>
   <commentList>
-    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{4CB254BE-00D1-40F2-8CA2-FEEC56060509}">
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{ABF08853-5593-46AB-BE86-313F60C60087}">
       <text>
         <r>
           <rPr>
@@ -280,15 +280,20 @@
             <family val="3"/>
             <charset val="134"/>
           </rPr>
+          <t>restaurant can create menu for itself</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
           <t xml:space="preserve">
-registeration page for restaurant
-Accpetence criteria:
-1. user information should be uploaded to database.</t>
+</t>
         </r>
-      </text>
-    </comment>
-    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{9F58866B-D075-4F2E-9882-E63F11BEA4AA}">
-      <text>
         <r>
           <rPr>
             <sz val="9"/>
@@ -297,15 +302,33 @@
             <family val="3"/>
             <charset val="134"/>
           </rPr>
+          <t>Acceptance critria:</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
           <t xml:space="preserve">
-Task2:
-registeration page for customer
-Accpetence criteria:
-1. user information should be uploaded to database.</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>1. restaurant can add meals by upload the picture, price and name of the meal.</t>
         </r>
       </text>
     </comment>
-    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{C038C97C-1387-4608-84DE-FA5F1C040391}">
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{5F8E571A-02B5-4AFD-B59A-3C4B069D15C6}">
       <text>
         <r>
           <rPr>
@@ -316,15 +339,25 @@
             <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>Task3:
-login page for restaurant
-Accpetence criteria:
-1. information match the database should return succeeded.
-2.information wrong then return errors.</t>
+          <t xml:space="preserve">Task1:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>restaurant can modify own menu
+Acceptence criteria:
+1.restaurant can change the name, price and the picture of meal.
+2. restaurant can completely delete a meal.</t>
         </r>
       </text>
     </comment>
-    <comment ref="D5" authorId="0" shapeId="0" xr:uid="{B52C074A-119A-4CF0-935D-65B3FF1D0C45}">
+    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{32E9E79D-CBFD-4809-A713-7460355A5A72}">
       <text>
         <r>
           <rPr>
@@ -335,29 +368,21 @@
             <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>Task4:
-login page for customer
-Accpetence criteria:
-1. information match the database should return succeeded.
-2.information wrong then return error.</t>
+          <t xml:space="preserve">Task 3:
+</t>
         </r>
-      </text>
-    </comment>
-    <comment ref="D6" authorId="0" shapeId="0" xr:uid="{36C41FD8-69D1-4C36-8355-99F954DFE0C1}">
-      <text>
         <r>
           <rPr>
-            <b/>
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="宋体"/>
             <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>Task5:
-information of restaurant should be displayed for customer.
-Accpetence criteria:
-1. information of each restaurant should be displayed corrently.</t>
+          <t xml:space="preserve">
+customer should be able to view the menu
+acceptance criteria:
+1. customer should be able to view the correct information of menu, including  price, name and picture of all meals</t>
         </r>
       </text>
     </comment>
@@ -366,7 +391,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="55">
   <si>
     <t>To Do (Sprint Backlog)</t>
   </si>
@@ -530,23 +555,15 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>Task 3: login for restaurant</t>
+    <t>Task 2: modify menu</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>Task 4: login for customer</t>
+    <t>Task 1: create menu</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>Task 2: regiseration for customer</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Task 1: regiseration for restaurant</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Task 5: display restaurant for customer</t>
+    <t>Task 3: display menu</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -908,6 +925,9 @@
                 <c:pt idx="1">
                   <c:v>1</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -921,6 +941,9 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
@@ -969,6 +992,9 @@
                 <c:pt idx="1">
                   <c:v>1</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -982,7 +1008,10 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6531,7 +6560,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -13570,10 +13599,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -13584,7 +13613,7 @@
     <col min="5" max="5" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -13599,28 +13628,18 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D2" s="37" t="s">
-        <v>55</v>
+      <c r="A2" s="37" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D3" s="37" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D4" s="37" t="s">
+      <c r="A3" s="37" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D5" s="37" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D6" s="37" t="s">
-        <v>56</v>
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="37" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -16682,7 +16701,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -16695,7 +16714,7 @@
     <col min="6" max="6" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="32" t="s">
         <v>38</v>
       </c>
@@ -16715,7 +16734,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="6">
         <v>0</v>
       </c>
@@ -16735,7 +16754,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -16752,15 +16771,30 @@
         <v>7</v>
       </c>
       <c r="F3" s="6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="6">
+        <v>2</v>
+      </c>
+      <c r="B4" s="6">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="F4" s="6"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E4">
+        <v>7</v>
+      </c>
+      <c r="F4" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="6"/>
       <c r="F5" s="6"/>
     </row>

</xml_diff>